<commit_message>
Board Detection Training Completed. board_detection.py object written
</commit_message>
<xml_diff>
--- a/Object-Design.xlsx
+++ b/Object-Design.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/artun/Desktop/CodePlay/Get-Chess-Board/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/artun/Desktop/Springboard/springboard/Get-Chess-Board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D724A42-A189-5E45-9019-5BB92B1464D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B1E8CA-695E-C043-81BF-EB909E29684A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{A7260B55-47C1-5E4A-B2E5-D898D15CF8E8}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
-  <si>
-    <t>Processing</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Object Classification</t>
   </si>
@@ -119,35 +116,9 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">YOLO </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - How do you detect a chess board? (What are inputs and outputs?)</t>
-    </r>
-  </si>
-  <si>
     <t>FEN</t>
   </si>
   <si>
-    <t>How do I make this operational? How does the user interface with this reasonably? What's the output?</t>
-  </si>
-  <si>
     <t xml:space="preserve">  ---many-to-one---&gt;  </t>
   </si>
   <si>
@@ -161,9 +132,6 @@
   </si>
   <si>
     <t>.predict(ndarray) -&gt; (miny,minx, maxy, maxy)</t>
-  </si>
-  <si>
-    <t>Can you implement it? - Decision TBD, maybe do the last parts</t>
   </si>
   <si>
     <t>Tkinter approach to Square Labeler Interface</t>
@@ -201,9 +169,6 @@
   </si>
   <si>
     <t>Control buttons for deleting rows and moving to next picture</t>
-  </si>
-  <si>
-    <t>Delete Box</t>
   </si>
   <si>
     <r>
@@ -230,6 +195,90 @@
   </si>
   <si>
     <t xml:space="preserve">Next </t>
+  </si>
+  <si>
+    <t>Delete BBox</t>
+  </si>
+  <si>
+    <t>draw_bbox(coords, label, canvas?)</t>
+  </si>
+  <si>
+    <t>Processing (Pick up Board)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Done YOLO </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - How do you detect a chess board? (What are inputs and outputs?)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Done</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Can you implement it? - Decision TBD, maybe do the last parts</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Done</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> How do I make this operational? How does the user interface with this reasonably? What's the output?</t>
+    </r>
+  </si>
+  <si>
+    <t>-&gt; Heroku (Streamlit) + Web -&gt; lichess.com</t>
+  </si>
+  <si>
+    <t>Lichess Analysis Board with FEN: https://lichess.org/analysis/3qkbnr/pppppppp/8/8/8/8/PPPPPPPP/3QKBNR%20w%20KQkq%20-%200%201</t>
   </si>
 </sst>
 </file>
@@ -821,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA307243-E608-CE43-ABB7-26EE0641C933}">
-  <dimension ref="A6:I47"/>
+  <dimension ref="A6:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -836,198 +885,199 @@
     <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:9" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:10" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="1" t="s">
+      <c r="G11" t="s">
         <v>2</v>
       </c>
-      <c r="G8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" t="s">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" t="s">
+    <row r="14" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:10" ht="64" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:9" ht="64" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>11</v>
-      </c>
       <c r="G16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.2">
       <c r="G18" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G20" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="3:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C34" s="10"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="12"/>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C35" s="13"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="15"/>
-    </row>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C36" s="13"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="15"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="12"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C37" s="13"/>
-      <c r="D37" s="17"/>
+      <c r="D37" s="14"/>
       <c r="E37" s="15"/>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C38" s="13"/>
-      <c r="D38" s="18"/>
+      <c r="D38" s="16"/>
       <c r="E38" s="15"/>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C39" s="13"/>
-      <c r="D39" s="14"/>
+      <c r="D39" s="17"/>
       <c r="E39" s="15"/>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C40" s="13"/>
-      <c r="D40" s="14"/>
+      <c r="D40" s="18"/>
       <c r="E40" s="15"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.2">
@@ -1046,37 +1096,47 @@
       <c r="E43" s="15"/>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C44" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D44" s="20"/>
-      <c r="E44" s="21" t="s">
-        <v>38</v>
-      </c>
+      <c r="C44" s="13"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="15"/>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C45" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D45" s="9"/>
-      <c r="E45" s="23" t="s">
-        <v>40</v>
-      </c>
+      <c r="C45" s="13"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="15"/>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C46" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D46" s="9"/>
-      <c r="E46" s="23" t="s">
-        <v>40</v>
+      <c r="C46" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" s="20"/>
+      <c r="E46" s="21" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C47" s="24"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="26" t="s">
-        <v>41</v>
+      <c r="C47" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C48" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" s="9"/>
+      <c r="E48" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C49" s="24"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="26" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Labeling Exposition. Started Objective and Demo. Rearranged directory structure. Corrected minor square csv mislabels
</commit_message>
<xml_diff>
--- a/Object-Design.xlsx
+++ b/Object-Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/artun/Desktop/Springboard/springboard/Get-Chess-Board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B1E8CA-695E-C043-81BF-EB909E29684A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FAC0C7-EB27-D940-8DCD-CBD936C68603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{A7260B55-47C1-5E4A-B2E5-D898D15CF8E8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>Object Classification</t>
   </si>
@@ -76,9 +76,6 @@
     <t>.check_train_data(train_dir)  #Brings up all data, enables demarking</t>
   </si>
   <si>
-    <t>Displays images in a directory with interface to label them</t>
-  </si>
-  <si>
     <t>Quick To Do</t>
   </si>
   <si>
@@ -132,33 +129,12 @@
   </si>
   <si>
     <t>.predict(ndarray) -&gt; (miny,minx, maxy, maxy)</t>
-  </si>
-  <si>
-    <t>Tkinter approach to Square Labeler Interface</t>
-  </si>
-  <si>
-    <t>draw_heading(SomeHeadigText)</t>
-  </si>
-  <si>
-    <t>draw_topline(list of vars as column sets)</t>
-  </si>
-  <si>
-    <t>draw_next() -&gt; click: save vars in main df; replace df with new df  if &lt;desired, name is END</t>
-  </si>
-  <si>
-    <t>draw_filters() -&gt; filter the main df for desired characteristics, include a filter button to activate draw_rows</t>
-  </si>
-  <si>
-    <t>Variable: {text='Header Text', type={'image','label'}, df_colname='colname in df', label_options=ATupleOfText</t>
   </si>
   <si>
     <t>Labelers
 (i-Screenshot, ii-Square)</t>
   </si>
   <si>
-    <t>draw_rows(list of vars as column sets, data table) -&gt; draws rows with choices as Radiobuttons</t>
-  </si>
-  <si>
     <t>Tkinter approach to Screenshot Labeler Interface</t>
   </si>
   <si>
@@ -275,17 +251,281 @@
     </r>
   </si>
   <si>
-    <t>-&gt; Heroku (Streamlit) + Web -&gt; lichess.com</t>
-  </si>
-  <si>
     <t>Lichess Analysis Board with FEN: https://lichess.org/analysis/3qkbnr/pppppppp/8/8/8/8/PPPPPPPP/3QKBNR%20w%20KQkq%20-%200%201</t>
+  </si>
+  <si>
+    <t>pc_pic / sq_color / pc_color / pc_type    / human_check</t>
+  </si>
+  <si>
+    <t>Make Estimates      |        Mark as Checked</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <r>
+      <t>♞       /     B</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">     / </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WE      / PR</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">BQKE /         </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">N                        </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>♔       /     B</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">     / B</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E      / PRNBQ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">E /         </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>♜       /     B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">     / BW</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">      / PRNBQK</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> /         Y</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>N</t>
+    </r>
+  </si>
+  <si>
+    <t>Displays images in a directory; has an interface to label them</t>
+  </si>
+  <si>
+    <t>Uses tkinter for cross-platform flexbility</t>
+  </si>
+  <si>
+    <t>i- Rough GUI for Screenshot Labeling</t>
+  </si>
+  <si>
+    <t>ii- Rough GUI for Square Labeling</t>
+  </si>
+  <si>
+    <t>-&gt; Eventually: Heroku (Streamlit) + Web -&gt; lichess.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -306,6 +546,18 @@
       <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -321,7 +573,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -508,11 +760,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -556,6 +839,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,15 +1174,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA307243-E608-CE43-ABB7-26EE0641C933}">
-  <dimension ref="A6:J49"/>
+  <dimension ref="A6:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
@@ -888,10 +1193,10 @@
     <row r="6" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:10" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>3</v>
@@ -900,7 +1205,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>5</v>
@@ -909,13 +1214,13 @@
         <v>0</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
@@ -926,12 +1231,12 @@
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
         <v>7</v>
@@ -939,7 +1244,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G11" t="s">
         <v>2</v>
@@ -964,7 +1269,7 @@
     <row r="14" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:10" ht="64" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -972,93 +1277,104 @@
         <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="G17" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
       <c r="G18" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>22</v>
-      </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>23</v>
-      </c>
       <c r="G20" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C29" t="s">
-        <v>31</v>
-      </c>
+      <c r="C29" s="10"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="12"/>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C30" t="s">
-        <v>38</v>
-      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="15"/>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C31" t="s">
-        <v>32</v>
-      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="15"/>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="3:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="15"/>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C33" s="13"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="15"/>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C34" s="13"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="15"/>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C35" s="13"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="15"/>
+    </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C36" s="10"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="12"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="15"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C37" s="13"/>
@@ -1067,79 +1383,115 @@
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C38" s="13"/>
-      <c r="D38" s="16"/>
+      <c r="D38" s="14"/>
       <c r="E38" s="15"/>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C39" s="13"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="15"/>
+      <c r="C39" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="20"/>
+      <c r="E39" s="21" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C40" s="13"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="15"/>
+      <c r="C40" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="23" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C41" s="13"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="15"/>
+      <c r="C41" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="9"/>
+      <c r="E41" s="23" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C42" s="13"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="15"/>
-    </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C43" s="13"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="15"/>
-    </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C44" s="13"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="15"/>
-    </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C45" s="13"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="15"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C46" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D46" s="20"/>
-      <c r="E46" s="21" t="s">
+      <c r="C46" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" s="29"/>
+      <c r="E46" s="30"/>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C47" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47" s="27"/>
+      <c r="E47" s="32"/>
+    </row>
+    <row r="48" spans="3:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C48" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48" s="27"/>
+      <c r="E48" s="32"/>
+    </row>
+    <row r="49" spans="3:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C49" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D49" s="27"/>
+      <c r="E49" s="32"/>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C50" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50" s="14"/>
+      <c r="E50" s="15"/>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C51" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" s="14"/>
+      <c r="E51" s="15"/>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C52" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52" s="14"/>
+      <c r="E52" s="15"/>
+    </row>
+    <row r="53" spans="3:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C53" s="33" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C47" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D47" s="9"/>
-      <c r="E47" s="23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C48" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D48" s="9"/>
-      <c r="E48" s="23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C49" s="24"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="26" t="s">
-        <v>36</v>
-      </c>
-    </row>
+      <c r="D53" s="34"/>
+      <c r="E53" s="35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="3:5" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Get Chess Board Part3a with demo training and detection with actual model. Added file name changes
</commit_message>
<xml_diff>
--- a/Object-Design.xlsx
+++ b/Object-Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/artun/Desktop/Springboard/springboard/Get-Chess-Board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FAC0C7-EB27-D940-8DCD-CBD936C68603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84002C11-267D-334A-B284-3190D0A37BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{A7260B55-47C1-5E4A-B2E5-D898D15CF8E8}"/>
   </bookViews>
@@ -839,9 +839,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -854,12 +854,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1174,11 +1174,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA307243-E608-CE43-ABB7-26EE0641C933}">
-  <dimension ref="A6:J58"/>
+  <dimension ref="A6:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1426,32 +1424,32 @@
       </c>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C46" s="28" t="s">
+      <c r="C46" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D46" s="29"/>
-      <c r="E46" s="30"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="32"/>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C47" s="31" t="s">
+      <c r="C47" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="D47" s="27"/>
-      <c r="E47" s="32"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="35"/>
     </row>
     <row r="48" spans="3:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C48" s="31" t="s">
+      <c r="C48" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D48" s="27"/>
-      <c r="E48" s="32"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="35"/>
     </row>
     <row r="49" spans="3:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C49" s="31" t="s">
+      <c r="C49" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D49" s="27"/>
-      <c r="E49" s="32"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="35"/>
     </row>
     <row r="50" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C50" s="13" t="s">
@@ -1475,16 +1473,14 @@
       <c r="E52" s="15"/>
     </row>
     <row r="53" spans="3:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="33" t="s">
+      <c r="C53" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D53" s="34"/>
-      <c r="E53" s="35" t="s">
+      <c r="D53" s="28"/>
+      <c r="E53" s="29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="3:5" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="3:5" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C46:E46"/>

</xml_diff>